<commit_message>
change: data and createDatabase.py, insertDatabase.py
</commit_message>
<xml_diff>
--- a/Dataset/staff.xlsx
+++ b/Dataset/staff.xlsx
@@ -96,9 +96,6 @@
     <t>An Giang</t>
   </si>
   <si>
-    <t>079534653344 ​</t>
-  </si>
-  <si>
     <t>TP. Ho Chi Minh</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Quang Nam</t>
+  </si>
+  <si>
+    <t>079534653344</t>
   </si>
 </sst>
 </file>
@@ -131,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -534,7 +534,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -572,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2">
@@ -587,7 +587,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2">
@@ -602,7 +602,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="2">
@@ -617,7 +617,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="2">
@@ -632,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="2">
@@ -647,7 +647,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="2">
@@ -662,7 +662,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="2">
@@ -692,7 +692,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2">
@@ -707,7 +707,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2">
@@ -722,7 +722,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2">
@@ -749,10 +749,10 @@
         <v>36678</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="2">

</xml_diff>